<commit_message>
Descomponer Excel - listo
</commit_message>
<xml_diff>
--- a/back-end/uploads/estudiantes.xlsx
+++ b/back-end/uploads/estudiantes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhunior\Desktop\ProyectoBaseDatos\proyecto-base-datos\back-end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhunior\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D83F249-99A7-4FD2-BFAD-21B5D3A7BB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6102DF1D-8D29-4A58-84E6-C750DB84E8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E3B6DDF-B402-4654-B968-21DF4C067117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>dni</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Palmeras Diaz</t>
+  </si>
+  <si>
+    <t>Pepito</t>
+  </si>
+  <si>
+    <t>Alima</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,35 +165,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -199,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -208,10 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -531,7 +510,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,80 +540,97 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>73332032</v>
+      <c r="A2" s="8">
+        <v>53332033</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6">
-        <v>37168</v>
-      </c>
-      <c r="E2" s="8" t="s">
+        <v>38172</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>69583654</v>
+      <c r="A3" s="8">
+        <v>73332032</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3" s="6">
-        <v>36652</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>10</v>
+        <v>37168</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>48856952</v>
+      <c r="A4" s="8">
+        <v>69583654</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6">
-        <v>37424</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
+        <v>36652</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>58456958</v>
+      <c r="A5" s="8">
+        <v>48856952</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="6">
-        <v>36950</v>
-      </c>
-      <c r="E5" s="9" t="s">
+        <v>37424</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>58456958</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6">
+        <v>36950</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>

</xml_diff>

<commit_message>
Registrar escuela - terminado
</commit_message>
<xml_diff>
--- a/back-end/uploads/estudiantes.xlsx
+++ b/back-end/uploads/estudiantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhunior\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFEE64B-4556-4B2B-AEED-66A814EE94C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EAF219-FDB2-42D5-82E7-DCB86189D3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E3B6DDF-B402-4654-B968-21DF4C067117}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +535,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>53332033</v>
+        <v>11111126</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>73332032</v>
+        <v>11111127</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -573,7 +573,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>69583654</v>
+        <v>11111128</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>48856952</v>
+        <v>11111129</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>58456958</v>
+        <v>11111130</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>

</xml_diff>